<commit_message>
modificacion de modulor vehiculos y modulo biblioteca
</commit_message>
<xml_diff>
--- a/Archivo_Importacion_Inventario_biblioteca.xlsx
+++ b/Archivo_Importacion_Inventario_biblioteca.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="86">
   <si>
     <t>SA5444</t>
   </si>
@@ -280,9 +280,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* \-??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
@@ -294,10 +294,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -309,7 +310,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -317,7 +318,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -328,14 +336,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -350,6 +350,21 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,22 +410,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -425,14 +432,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -447,187 +447,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,8 +644,34 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -661,26 +687,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,21 +715,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -738,29 +729,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -770,121 +770,121 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1219,8 +1219,8 @@
   <sheetPr/>
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1234,6 +1234,7 @@
     <col min="7" max="7" width="4.28571428571429" customWidth="1"/>
     <col min="9" max="9" width="20.5714285714286" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="16" max="16" width="10.2857142857143"/>
     <col min="17" max="20" width="11.4285714285714"/>
   </cols>
   <sheetData>
@@ -2529,7 +2530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" ht="45" spans="1:22">
+    <row r="20" ht="45" spans="1:21">
       <c r="A20">
         <v>1263</v>
       </c>
@@ -2570,13 +2571,13 @@
         <v>69</v>
       </c>
       <c r="N20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O20" t="s">
-        <v>10</v>
-      </c>
-      <c r="P20" t="s">
         <v>70</v>
+      </c>
+      <c r="P20" s="1">
+        <v>44337</v>
       </c>
       <c r="Q20" s="1">
         <v>44337</v>
@@ -2587,17 +2588,14 @@
       <c r="S20" s="1">
         <v>44337</v>
       </c>
-      <c r="T20" s="1">
-        <v>44337</v>
-      </c>
-      <c r="U20" s="2" t="s">
+      <c r="T20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V20" t="s">
+      <c r="U20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" ht="45" spans="1:22">
+    <row r="21" ht="45" spans="1:21">
       <c r="A21">
         <v>1264</v>
       </c>
@@ -2638,13 +2636,13 @@
         <v>72</v>
       </c>
       <c r="N21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O21" t="s">
-        <v>10</v>
-      </c>
-      <c r="P21" t="s">
         <v>73</v>
+      </c>
+      <c r="P21" s="1">
+        <v>44338</v>
       </c>
       <c r="Q21" s="1">
         <v>44338</v>
@@ -2655,17 +2653,14 @@
       <c r="S21" s="1">
         <v>44338</v>
       </c>
-      <c r="T21" s="1">
-        <v>44338</v>
-      </c>
-      <c r="U21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V21" t="s">
+      <c r="U21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" ht="45" spans="1:22">
+    <row r="22" ht="45" spans="1:21">
       <c r="A22">
         <v>1265</v>
       </c>
@@ -2706,13 +2701,13 @@
         <v>75</v>
       </c>
       <c r="N22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O22" t="s">
-        <v>10</v>
-      </c>
-      <c r="P22" t="s">
         <v>76</v>
+      </c>
+      <c r="P22" s="1">
+        <v>44339</v>
       </c>
       <c r="Q22" s="1">
         <v>44339</v>
@@ -2723,17 +2718,14 @@
       <c r="S22" s="1">
         <v>44339</v>
       </c>
-      <c r="T22" s="1">
-        <v>44339</v>
-      </c>
-      <c r="U22" s="2" t="s">
+      <c r="T22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V22" t="s">
+      <c r="U22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" ht="45" spans="1:22">
+    <row r="23" ht="45" spans="1:21">
       <c r="A23">
         <v>1266</v>
       </c>
@@ -2774,13 +2766,13 @@
         <v>78</v>
       </c>
       <c r="N23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>10</v>
-      </c>
-      <c r="P23" t="s">
         <v>79</v>
+      </c>
+      <c r="P23" s="1">
+        <v>44340</v>
       </c>
       <c r="Q23" s="1">
         <v>44340</v>
@@ -2791,17 +2783,14 @@
       <c r="S23" s="1">
         <v>44340</v>
       </c>
-      <c r="T23" s="1">
-        <v>44340</v>
-      </c>
-      <c r="U23" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V23" t="s">
+      <c r="U23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" ht="45" spans="1:22">
+    <row r="24" ht="45" spans="1:21">
       <c r="A24">
         <v>1267</v>
       </c>
@@ -2842,13 +2831,13 @@
         <v>81</v>
       </c>
       <c r="N24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>10</v>
-      </c>
-      <c r="P24" t="s">
         <v>82</v>
+      </c>
+      <c r="P24" s="1">
+        <v>44341</v>
       </c>
       <c r="Q24" s="1">
         <v>44341</v>
@@ -2859,17 +2848,14 @@
       <c r="S24" s="1">
         <v>44341</v>
       </c>
-      <c r="T24" s="1">
-        <v>44341</v>
-      </c>
-      <c r="U24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V24" t="s">
+      <c r="U24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" ht="45" spans="1:22">
+    <row r="25" ht="45" spans="1:21">
       <c r="A25">
         <v>1268</v>
       </c>
@@ -2910,13 +2896,13 @@
         <v>84</v>
       </c>
       <c r="N25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O25" t="s">
-        <v>10</v>
-      </c>
-      <c r="P25" t="s">
         <v>85</v>
+      </c>
+      <c r="P25" s="1">
+        <v>44342</v>
       </c>
       <c r="Q25" s="1">
         <v>44342</v>
@@ -2927,13 +2913,10 @@
       <c r="S25" s="1">
         <v>44342</v>
       </c>
-      <c r="T25" s="1">
-        <v>44342</v>
-      </c>
-      <c r="U25" s="2" t="s">
+      <c r="T25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="V25" t="s">
+      <c r="U25" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>